<commit_message>
update requirements and readme
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,11 +511,7 @@
           <t>Based on the transcript provided, it appears that your experience involved assisting a young man named Handri, who is 19 years old and intoxicated. You helped him with his mayo, provided him with a hotel reservation, and offered basic first aid in the form of a water bottle and vomit bag due to his wobbly voice and imbalance. Your experience involved quick thinking and providing immediate care to someone in need.</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4354,6 +4350,44 @@
         </is>
       </c>
       <c r="H103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>18-25</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Speech, Behavior</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Transport, Friends</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Water</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Based on the transcript, it seems like your experience involved assisting a drunk individual who was with his friends. You took the initiative to provide him with a water bottle to help him sober up. Your actions demonstrate care and responsibility towards the well-being of others in a potentially risky situation.</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>